<commit_message>
Event and Menu relationship, import menu.
</commit_message>
<xml_diff>
--- a/fixture/src/main/java/domainapp/fixture/scenarios/spreadsheets/EventImport.xlsx
+++ b/fixture/src/main/java/domainapp/fixture/scenarios/spreadsheets/EventImport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -31,15 +31,15 @@
   </si>
   <si>
     <t>Xmas Party</t>
+  </si>
+  <si>
+    <t>Non Member Supplement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,9 +71,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,14 +379,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -396,33 +396,42 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>42186</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>42308</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="3">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>42356</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="3">
+        <v>3.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
menus now have items
</commit_message>
<xml_diff>
--- a/fixture/src/main/java/domainapp/fixture/scenarios/spreadsheets/EventImport.xlsx
+++ b/fixture/src/main/java/domainapp/fixture/scenarios/spreadsheets/EventImport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,36 @@
   </si>
   <si>
     <t>Non Member Supplement</t>
+  </si>
+  <si>
+    <t>Ingredient</t>
+  </si>
+  <si>
+    <t>Wurst</t>
+  </si>
+  <si>
+    <t>Member Price</t>
+  </si>
+  <si>
+    <t>Brochette</t>
+  </si>
+  <si>
+    <t>Steak</t>
+  </si>
+  <si>
+    <t>Bearnaise Sauce</t>
+  </si>
+  <si>
+    <t>Mushroom Sauce</t>
+  </si>
+  <si>
+    <t>Pepper Sauce</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>Trout</t>
   </si>
 </sst>
 </file>
@@ -375,11 +405,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,9 +417,11 @@
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,8 +431,14 @@
       <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -410,26 +448,116 @@
       <c r="C2" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B10" s="1">
         <v>42308</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C10" s="3">
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B11" s="1">
         <v>42356</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C11" s="3">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>